<commit_message>
As of March 23,2018 - 3:50AM
</commit_message>
<xml_diff>
--- a/ARB2.xlsx
+++ b/ARB2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher Jorge\Documents\NetBeansProjects\DARBMS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769B7984-5220-4FDB-B0DA-044D386249C4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>First Name</t>
   </si>
@@ -108,9 +114,6 @@
     <t>Tomato,Cabbage,Corn</t>
   </si>
   <si>
-    <t>Tertiary - Undergraduate</t>
-  </si>
-  <si>
     <t>Unit No. Street</t>
   </si>
   <si>
@@ -186,18 +189,12 @@
     <t>Noel Bryant</t>
   </si>
   <si>
-    <t>Primary</t>
-  </si>
-  <si>
     <t>Rey Christian Lopez Gamboa</t>
   </si>
   <si>
     <t>Junior Duncan</t>
   </si>
   <si>
-    <t>Secondary</t>
-  </si>
-  <si>
     <t>Shareef Mohammed</t>
   </si>
   <si>
@@ -208,12 +205,48 @@
   </si>
   <si>
     <t>Donovan Mitchell</t>
+  </si>
+  <si>
+    <t>Crop Type</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Wife</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Sister</t>
+  </si>
+  <si>
+    <t>College Level</t>
+  </si>
+  <si>
+    <t>Vocational</t>
+  </si>
+  <si>
+    <t>Rice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +320,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -295,6 +328,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -343,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,9 +412,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,6 +464,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -586,11 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +674,7 @@
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -623,19 +694,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>5</v>
@@ -667,19 +738,19 @@
         <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="L2">
         <v>123000</v>
@@ -708,19 +779,19 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="L3">
         <v>124222</v>
@@ -749,19 +820,19 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="L4">
         <v>3452</v>
@@ -790,19 +861,19 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="L5">
         <v>232323</v>
@@ -818,11 +889,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,106 +901,161 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3">
+        <v>35691</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3">
+        <v>34625</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3">
+        <v>24107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="3">
+        <v>27679</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="3">
+        <v>34711</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="3">
+        <v>43152</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43187</v>
+      </c>
+      <c r="D2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="3">
-        <v>35691</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="3">
-        <v>34625</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="3">
-        <v>24107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="3">
-        <v>27679</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="3">
-        <v>34711</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>